<commit_message>
Updated metadata file according to slack message by Thomas
</commit_message>
<xml_diff>
--- a/PL2/PL2-parser/src/main/resources/metadata.xlsx
+++ b/PL2/PL2-parser/src/main/resources/metadata.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faris\Documents\Sourcetree\PL2-2016\PL2\PL2-parser\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="805"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15540" tabRatio="805"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1589,68 +1594,68 @@
     </xf>
   </cellXfs>
   <cellStyles count="125">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1713,10 +1718,18 @@
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2044,39 +2057,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA554"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G282" workbookViewId="0">
-      <selection activeCell="Z316" sqref="Z1:Z1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="X220" sqref="X220"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.375" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="3" customFormat="1" ht="50">
+    <row r="1" spans="1:27" s="3" customFormat="1" ht="73.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>61</v>
       </c>
@@ -2159,7 +2172,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>94</v>
       </c>
@@ -2242,7 +2255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>99</v>
       </c>
@@ -2325,7 +2338,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>102</v>
       </c>
@@ -2408,7 +2421,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>104</v>
       </c>
@@ -2491,7 +2504,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>105</v>
       </c>
@@ -2574,7 +2587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>107</v>
       </c>
@@ -2657,7 +2670,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>108</v>
       </c>
@@ -2740,7 +2753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>109</v>
       </c>
@@ -2823,7 +2836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>110</v>
       </c>
@@ -2906,7 +2919,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>113</v>
       </c>
@@ -2989,7 +3002,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>115</v>
       </c>
@@ -3072,7 +3085,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>118</v>
       </c>
@@ -3155,7 +3168,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>120</v>
       </c>
@@ -3238,7 +3251,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>121</v>
       </c>
@@ -3321,7 +3334,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>122</v>
       </c>
@@ -3404,7 +3417,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>123</v>
       </c>
@@ -3487,7 +3500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>124</v>
       </c>
@@ -3570,7 +3583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>127</v>
       </c>
@@ -3653,7 +3666,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>130</v>
       </c>
@@ -3736,7 +3749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>131</v>
       </c>
@@ -3819,7 +3832,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>133</v>
       </c>
@@ -3902,7 +3915,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>134</v>
       </c>
@@ -3985,7 +3998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>135</v>
       </c>
@@ -4068,7 +4081,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>136</v>
       </c>
@@ -4151,7 +4164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>137</v>
       </c>
@@ -4234,7 +4247,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>140</v>
       </c>
@@ -4317,7 +4330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>142</v>
       </c>
@@ -4400,7 +4413,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>143</v>
       </c>
@@ -4483,7 +4496,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>146</v>
       </c>
@@ -4566,7 +4579,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>147</v>
       </c>
@@ -4649,7 +4662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>148</v>
       </c>
@@ -4732,7 +4745,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>151</v>
       </c>
@@ -4815,7 +4828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:27">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>152</v>
       </c>
@@ -4898,7 +4911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:27">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>153</v>
       </c>
@@ -4981,7 +4994,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:27">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>154</v>
       </c>
@@ -5064,7 +5077,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:27">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>158</v>
       </c>
@@ -5147,7 +5160,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>159</v>
       </c>
@@ -5230,7 +5243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:27">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>161</v>
       </c>
@@ -5313,7 +5326,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:27">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>163</v>
       </c>
@@ -5396,7 +5409,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:27">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>164</v>
       </c>
@@ -5479,7 +5492,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:27">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>66</v>
       </c>
@@ -5562,7 +5575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:27">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>191</v>
       </c>
@@ -5645,7 +5658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:27" s="3" customFormat="1" ht="50">
+    <row r="44" spans="1:27" s="3" customFormat="1" ht="73.5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>61</v>
       </c>
@@ -5728,7 +5741,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="45" spans="1:27">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>192</v>
       </c>
@@ -5811,7 +5824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:27">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>67</v>
       </c>
@@ -5894,7 +5907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:27">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>194</v>
       </c>
@@ -5977,7 +5990,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:27">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>75</v>
       </c>
@@ -6060,7 +6073,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:27">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>78</v>
       </c>
@@ -6143,7 +6156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:27">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>200</v>
       </c>
@@ -6226,7 +6239,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:27">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>88</v>
       </c>
@@ -6309,7 +6322,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:27">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>89</v>
       </c>
@@ -6392,7 +6405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:27">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>204</v>
       </c>
@@ -6475,7 +6488,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:27">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>201</v>
       </c>
@@ -6558,7 +6571,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:27">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>203</v>
       </c>
@@ -6641,7 +6654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:27">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>90</v>
       </c>
@@ -6724,7 +6737,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:27">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>91</v>
       </c>
@@ -6807,7 +6820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:27">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>92</v>
       </c>
@@ -6890,7 +6903,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:27">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>93</v>
       </c>
@@ -6973,7 +6986,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:27">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>350</v>
       </c>
@@ -7056,7 +7069,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:27">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>351</v>
       </c>
@@ -7139,7 +7152,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:27">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>366</v>
       </c>
@@ -7222,7 +7235,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:27">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
         <v>367</v>
       </c>
@@ -7305,7 +7318,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:27">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>368</v>
       </c>
@@ -7388,7 +7401,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:27">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
         <v>356</v>
       </c>
@@ -7471,7 +7484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:27">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>358</v>
       </c>
@@ -7554,7 +7567,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:27">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>370</v>
       </c>
@@ -7637,7 +7650,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:27">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
         <v>359</v>
       </c>
@@ -7720,7 +7733,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:27">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
         <v>360</v>
       </c>
@@ -7803,7 +7816,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:27">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>361</v>
       </c>
@@ -7886,7 +7899,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:27">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>362</v>
       </c>
@@ -7969,7 +7982,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:27">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
         <v>371</v>
       </c>
@@ -8052,7 +8065,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:27">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
         <v>372</v>
       </c>
@@ -8135,7 +8148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:27">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
         <v>380</v>
       </c>
@@ -8218,7 +8231,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:27">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
         <v>373</v>
       </c>
@@ -8301,7 +8314,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:27">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
         <v>374</v>
       </c>
@@ -8384,7 +8397,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:27">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
         <v>375</v>
       </c>
@@ -8467,7 +8480,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:27">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
         <v>379</v>
       </c>
@@ -8550,7 +8563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:27">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>363</v>
       </c>
@@ -8633,7 +8646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:27">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
         <v>376</v>
       </c>
@@ -8716,7 +8729,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:27">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
         <v>377</v>
       </c>
@@ -8799,7 +8812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:27">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
         <v>378</v>
       </c>
@@ -8882,7 +8895,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:27">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
         <v>364</v>
       </c>
@@ -8965,7 +8978,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:27">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
         <v>365</v>
       </c>
@@ -9048,7 +9061,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:27">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
         <v>252</v>
       </c>
@@ -9131,7 +9144,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:27">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
         <v>253</v>
       </c>
@@ -9214,7 +9227,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:27" s="3" customFormat="1" ht="50">
+    <row r="87" spans="1:27" s="3" customFormat="1" ht="73.5" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>61</v>
       </c>
@@ -9297,7 +9310,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="88" spans="1:27">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
         <v>254</v>
       </c>
@@ -9380,7 +9393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:27">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
         <v>255</v>
       </c>
@@ -9463,7 +9476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:27">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
         <v>256</v>
       </c>
@@ -9546,7 +9559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:27">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
         <v>257</v>
       </c>
@@ -9629,7 +9642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:27">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
         <v>260</v>
       </c>
@@ -9712,7 +9725,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:27">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
         <v>261</v>
       </c>
@@ -9795,7 +9808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:27">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
         <v>262</v>
       </c>
@@ -9878,7 +9891,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:27">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
         <v>263</v>
       </c>
@@ -9961,7 +9974,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="1:27">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="s">
         <v>264</v>
       </c>
@@ -10044,7 +10057,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:27">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
         <v>303</v>
       </c>
@@ -10127,7 +10140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:27">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
         <v>265</v>
       </c>
@@ -10210,7 +10223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:27">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
         <v>268</v>
       </c>
@@ -10293,7 +10306,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:27">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
         <v>269</v>
       </c>
@@ -10376,7 +10389,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:27">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
         <v>272</v>
       </c>
@@ -10459,7 +10472,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:27">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="s">
         <v>306</v>
       </c>
@@ -10542,7 +10555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:27">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
         <v>308</v>
       </c>
@@ -10625,7 +10638,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="1:27">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
         <v>309</v>
       </c>
@@ -10708,7 +10721,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:27">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" s="12" t="s">
         <v>310</v>
       </c>
@@ -10791,7 +10804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:27">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="s">
         <v>328</v>
       </c>
@@ -10874,7 +10887,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:27">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
         <v>329</v>
       </c>
@@ -10957,7 +10970,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="1:27">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" s="12" t="s">
         <v>331</v>
       </c>
@@ -11040,7 +11053,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="1:27">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
         <v>332</v>
       </c>
@@ -11123,7 +11136,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:27">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" s="12" t="s">
         <v>334</v>
       </c>
@@ -11206,7 +11219,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="111" spans="1:27">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" s="12" t="s">
         <v>335</v>
       </c>
@@ -11289,7 +11302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="1:27">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" s="12" t="s">
         <v>337</v>
       </c>
@@ -11372,7 +11385,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:27">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A113" s="12" t="s">
         <v>339</v>
       </c>
@@ -11455,7 +11468,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="114" spans="1:27">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A114" s="12" t="s">
         <v>340</v>
       </c>
@@ -11538,7 +11551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="115" spans="1:27">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A115" s="12" t="s">
         <v>343</v>
       </c>
@@ -11621,7 +11634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="116" spans="1:27">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A116" s="12" t="s">
         <v>344</v>
       </c>
@@ -11704,7 +11717,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="117" spans="1:27">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
         <v>346</v>
       </c>
@@ -11787,7 +11800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="118" spans="1:27">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
         <v>348</v>
       </c>
@@ -11870,7 +11883,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="1:27">
+    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
         <v>273</v>
       </c>
@@ -11953,7 +11966,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="120" spans="1:27">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
         <v>274</v>
       </c>
@@ -12036,7 +12049,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="121" spans="1:27">
+    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A121" s="12" t="s">
         <v>275</v>
       </c>
@@ -12119,7 +12132,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:27">
+    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
         <v>276</v>
       </c>
@@ -12202,7 +12215,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="123" spans="1:27">
+    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
         <v>277</v>
       </c>
@@ -12285,7 +12298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:27">
+    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A124" s="12" t="s">
         <v>278</v>
       </c>
@@ -12368,7 +12381,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="125" spans="1:27">
+    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A125" s="12" t="s">
         <v>279</v>
       </c>
@@ -12451,7 +12464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="1:27">
+    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
         <v>283</v>
       </c>
@@ -12534,7 +12547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="127" spans="1:27">
+    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A127" s="12" t="s">
         <v>284</v>
       </c>
@@ -12617,7 +12630,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="128" spans="1:27">
+    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A128" s="12" t="s">
         <v>285</v>
       </c>
@@ -12700,7 +12713,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:27">
+    <row r="129" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
         <v>289</v>
       </c>
@@ -12783,7 +12796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="130" spans="1:27" s="3" customFormat="1" ht="50">
+    <row r="130" spans="1:27" s="3" customFormat="1" ht="73.5" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>61</v>
       </c>
@@ -12866,7 +12879,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="131" spans="1:27">
+    <row r="131" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A131" s="12" t="s">
         <v>292</v>
       </c>
@@ -12949,7 +12962,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="132" spans="1:27">
+    <row r="132" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A132" s="12" t="s">
         <v>293</v>
       </c>
@@ -13032,7 +13045,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="133" spans="1:27">
+    <row r="133" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A133" s="12" t="s">
         <v>294</v>
       </c>
@@ -13115,7 +13128,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="134" spans="1:27">
+    <row r="134" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A134" s="12" t="s">
         <v>296</v>
       </c>
@@ -13198,7 +13211,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="135" spans="1:27">
+    <row r="135" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
         <v>298</v>
       </c>
@@ -13281,7 +13294,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:27">
+    <row r="136" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A136" s="12" t="s">
         <v>299</v>
       </c>
@@ -13364,7 +13377,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="1:27">
+    <row r="137" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A137" s="12" t="s">
         <v>300</v>
       </c>
@@ -13447,7 +13460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="138" spans="1:27">
+    <row r="138" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A138" s="12" t="s">
         <v>301</v>
       </c>
@@ -13530,7 +13543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="139" spans="1:27">
+    <row r="139" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A139" s="12" t="s">
         <v>302</v>
       </c>
@@ -13613,7 +13626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="140" spans="1:27">
+    <row r="140" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A140" s="12" t="s">
         <v>98</v>
       </c>
@@ -13696,7 +13709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="141" spans="1:27">
+    <row r="141" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A141" s="12" t="s">
         <v>101</v>
       </c>
@@ -13779,7 +13792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="142" spans="1:27">
+    <row r="142" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A142" s="12" t="s">
         <v>103</v>
       </c>
@@ -13862,7 +13875,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="143" spans="1:27">
+    <row r="143" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A143" s="12" t="s">
         <v>111</v>
       </c>
@@ -13945,7 +13958,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="144" spans="1:27">
+    <row r="144" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A144" s="12" t="s">
         <v>116</v>
       </c>
@@ -14028,7 +14041,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="145" spans="1:27">
+    <row r="145" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A145" s="12" t="s">
         <v>126</v>
       </c>
@@ -14111,7 +14124,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="146" spans="1:27">
+    <row r="146" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A146" s="12" t="s">
         <v>128</v>
       </c>
@@ -14194,7 +14207,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="147" spans="1:27">
+    <row r="147" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A147" s="12" t="s">
         <v>129</v>
       </c>
@@ -14277,7 +14290,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="148" spans="1:27">
+    <row r="148" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A148" s="12" t="s">
         <v>138</v>
       </c>
@@ -14360,7 +14373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="149" spans="1:27">
+    <row r="149" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
         <v>141</v>
       </c>
@@ -14443,7 +14456,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="150" spans="1:27">
+    <row r="150" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A150" s="12" t="s">
         <v>144</v>
       </c>
@@ -14526,7 +14539,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="151" spans="1:27">
+    <row r="151" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A151" s="12" t="s">
         <v>150</v>
       </c>
@@ -14609,7 +14622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="152" spans="1:27">
+    <row r="152" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A152" s="12" t="s">
         <v>155</v>
       </c>
@@ -14692,7 +14705,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="153" spans="1:27">
+    <row r="153" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A153" s="12" t="s">
         <v>157</v>
       </c>
@@ -14775,7 +14788,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="154" spans="1:27">
+    <row r="154" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A154" s="12" t="s">
         <v>160</v>
       </c>
@@ -14858,7 +14871,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="155" spans="1:27">
+    <row r="155" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A155" s="12" t="s">
         <v>162</v>
       </c>
@@ -14941,7 +14954,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="156" spans="1:27">
+    <row r="156" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A156" s="12" t="s">
         <v>166</v>
       </c>
@@ -15024,7 +15037,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:27">
+    <row r="157" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A157" s="12" t="s">
         <v>167</v>
       </c>
@@ -15107,7 +15120,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="158" spans="1:27">
+    <row r="158" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A158" s="12" t="s">
         <v>169</v>
       </c>
@@ -15190,7 +15203,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="159" spans="1:27">
+    <row r="159" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A159" s="12" t="s">
         <v>198</v>
       </c>
@@ -15273,7 +15286,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="160" spans="1:27">
+    <row r="160" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A160" s="12" t="s">
         <v>207</v>
       </c>
@@ -15356,7 +15369,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="1:27">
+    <row r="161" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A161" s="12" t="s">
         <v>208</v>
       </c>
@@ -15439,7 +15452,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="162" spans="1:27">
+    <row r="162" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A162" s="12" t="s">
         <v>424</v>
       </c>
@@ -15522,7 +15535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="163" spans="1:27">
+    <row r="163" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A163" s="12" t="s">
         <v>221</v>
       </c>
@@ -15605,7 +15618,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="164" spans="1:27">
+    <row r="164" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A164" s="12" t="s">
         <v>233</v>
       </c>
@@ -15688,7 +15701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="165" spans="1:27">
+    <row r="165" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A165" s="12" t="s">
         <v>352</v>
       </c>
@@ -15771,7 +15784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="166" spans="1:27">
+    <row r="166" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A166" s="12" t="s">
         <v>353</v>
       </c>
@@ -15854,7 +15867,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="167" spans="1:27">
+    <row r="167" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A167" s="12" t="s">
         <v>369</v>
       </c>
@@ -15937,7 +15950,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="168" spans="1:27">
+    <row r="168" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A168" s="12" t="s">
         <v>354</v>
       </c>
@@ -16020,7 +16033,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="169" spans="1:27">
+    <row r="169" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A169" s="12" t="s">
         <v>355</v>
       </c>
@@ -16103,7 +16116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="170" spans="1:27">
+    <row r="170" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A170" s="12" t="s">
         <v>258</v>
       </c>
@@ -16186,7 +16199,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="171" spans="1:27">
+    <row r="171" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A171" s="12" t="s">
         <v>259</v>
       </c>
@@ -16269,7 +16282,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="172" spans="1:27">
+    <row r="172" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A172" s="12" t="s">
         <v>266</v>
       </c>
@@ -16352,7 +16365,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="173" spans="1:27" s="3" customFormat="1" ht="50">
+    <row r="173" spans="1:27" s="3" customFormat="1" ht="73.5" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
         <v>61</v>
       </c>
@@ -16435,7 +16448,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="174" spans="1:27">
+    <row r="174" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A174" s="12" t="s">
         <v>267</v>
       </c>
@@ -16506,7 +16519,7 @@
         <v>55</v>
       </c>
       <c r="X174" s="9" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="Y174" s="11" t="s">
         <v>432</v>
@@ -16518,7 +16531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="175" spans="1:27">
+    <row r="175" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A175" s="12" t="s">
         <v>270</v>
       </c>
@@ -16601,7 +16614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="1:27">
+    <row r="176" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A176" s="12" t="s">
         <v>271</v>
       </c>
@@ -16684,7 +16697,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="177" spans="1:27">
+    <row r="177" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A177" s="12" t="s">
         <v>304</v>
       </c>
@@ -16767,7 +16780,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="178" spans="1:27">
+    <row r="178" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A178" s="12" t="s">
         <v>305</v>
       </c>
@@ -16850,7 +16863,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="179" spans="1:27">
+    <row r="179" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A179" s="12" t="s">
         <v>307</v>
       </c>
@@ -16933,7 +16946,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="180" spans="1:27">
+    <row r="180" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A180" s="12" t="s">
         <v>311</v>
       </c>
@@ -17016,7 +17029,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="181" spans="1:27">
+    <row r="181" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A181" s="12" t="s">
         <v>312</v>
       </c>
@@ -17099,7 +17112,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="182" spans="1:27">
+    <row r="182" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A182" s="12" t="s">
         <v>338</v>
       </c>
@@ -17182,7 +17195,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="183" spans="1:27">
+    <row r="183" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A183" s="12" t="s">
         <v>341</v>
       </c>
@@ -17265,7 +17278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="184" spans="1:27">
+    <row r="184" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A184" s="12" t="s">
         <v>342</v>
       </c>
@@ -17348,7 +17361,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="185" spans="1:27">
+    <row r="185" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A185" s="12" t="s">
         <v>345</v>
       </c>
@@ -17431,7 +17444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="186" spans="1:27">
+    <row r="186" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A186" s="12" t="s">
         <v>347</v>
       </c>
@@ -17514,7 +17527,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="187" spans="1:27">
+    <row r="187" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A187" s="12" t="s">
         <v>288</v>
       </c>
@@ -17597,7 +17610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="188" spans="1:27">
+    <row r="188" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A188" s="12" t="s">
         <v>290</v>
       </c>
@@ -17680,7 +17693,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="189" spans="1:27">
+    <row r="189" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A189" s="12" t="s">
         <v>291</v>
       </c>
@@ -17763,7 +17776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="190" spans="1:27">
+    <row r="190" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A190" s="12" t="s">
         <v>297</v>
       </c>
@@ -17846,7 +17859,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="191" spans="1:27">
+    <row r="191" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A191" s="12" t="s">
         <v>95</v>
       </c>
@@ -17929,7 +17942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="192" spans="1:27">
+    <row r="192" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A192" s="12" t="s">
         <v>96</v>
       </c>
@@ -18012,7 +18025,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="193" spans="1:27">
+    <row r="193" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A193" s="12" t="s">
         <v>100</v>
       </c>
@@ -18095,7 +18108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="194" spans="1:27">
+    <row r="194" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A194" s="12" t="s">
         <v>114</v>
       </c>
@@ -18178,7 +18191,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="195" spans="1:27">
+    <row r="195" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A195" s="12" t="s">
         <v>119</v>
       </c>
@@ -18261,7 +18274,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="196" spans="1:27">
+    <row r="196" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A196" s="12" t="s">
         <v>139</v>
       </c>
@@ -18344,7 +18357,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="197" spans="1:27">
+    <row r="197" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A197" s="12" t="s">
         <v>145</v>
       </c>
@@ -18427,7 +18440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="198" spans="1:27">
+    <row r="198" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A198" s="12" t="s">
         <v>149</v>
       </c>
@@ -18510,7 +18523,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="199" spans="1:27">
+    <row r="199" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A199" s="12" t="s">
         <v>156</v>
       </c>
@@ -18593,7 +18606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="200" spans="1:27">
+    <row r="200" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A200" s="12" t="s">
         <v>168</v>
       </c>
@@ -18676,7 +18689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="201" spans="1:27">
+    <row r="201" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A201" s="12" t="s">
         <v>170</v>
       </c>
@@ -18759,7 +18772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="202" spans="1:27">
+    <row r="202" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A202" s="12" t="s">
         <v>171</v>
       </c>
@@ -18842,7 +18855,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="203" spans="1:27">
+    <row r="203" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A203" s="12" t="s">
         <v>172</v>
       </c>
@@ -18925,7 +18938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="204" spans="1:27">
+    <row r="204" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A204" s="12" t="s">
         <v>173</v>
       </c>
@@ -19008,7 +19021,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="205" spans="1:27">
+    <row r="205" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A205" s="12" t="s">
         <v>174</v>
       </c>
@@ -19091,7 +19104,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="206" spans="1:27">
+    <row r="206" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A206" s="12" t="s">
         <v>175</v>
       </c>
@@ -19174,7 +19187,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="207" spans="1:27">
+    <row r="207" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A207" s="12" t="s">
         <v>176</v>
       </c>
@@ -19257,7 +19270,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="208" spans="1:27">
+    <row r="208" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A208" s="12" t="s">
         <v>177</v>
       </c>
@@ -19340,7 +19353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="209" spans="1:27">
+    <row r="209" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A209" s="12" t="s">
         <v>178</v>
       </c>
@@ -19423,7 +19436,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="210" spans="1:27">
+    <row r="210" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A210" s="12" t="s">
         <v>179</v>
       </c>
@@ -19506,7 +19519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="211" spans="1:27">
+    <row r="211" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A211" s="12" t="s">
         <v>180</v>
       </c>
@@ -19589,7 +19602,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="212" spans="1:27">
+    <row r="212" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A212" s="12" t="s">
         <v>181</v>
       </c>
@@ -19672,7 +19685,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="213" spans="1:27">
+    <row r="213" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A213" s="12" t="s">
         <v>182</v>
       </c>
@@ -19755,7 +19768,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="214" spans="1:27">
+    <row r="214" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A214" s="12" t="s">
         <v>183</v>
       </c>
@@ -19838,7 +19851,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="215" spans="1:27">
+    <row r="215" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A215" s="12" t="s">
         <v>205</v>
       </c>
@@ -19921,7 +19934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="216" spans="1:27" s="3" customFormat="1" ht="50">
+    <row r="216" spans="1:27" s="3" customFormat="1" ht="73.5" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
         <v>61</v>
       </c>
@@ -20004,7 +20017,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="217" spans="1:27">
+    <row r="217" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A217" s="12" t="s">
         <v>418</v>
       </c>
@@ -20087,7 +20100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="218" spans="1:27">
+    <row r="218" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A218" s="12" t="s">
         <v>206</v>
       </c>
@@ -20170,7 +20183,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="219" spans="1:27">
+    <row r="219" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A219" s="12" t="s">
         <v>419</v>
       </c>
@@ -20253,7 +20266,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="220" spans="1:27">
+    <row r="220" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A220" s="12" t="s">
         <v>420</v>
       </c>
@@ -20324,7 +20337,7 @@
         <v>2</v>
       </c>
       <c r="X220" s="9" t="s">
-        <v>2</v>
+        <v>408</v>
       </c>
       <c r="Y220" s="11" t="s">
         <v>399</v>
@@ -20336,7 +20349,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="221" spans="1:27">
+    <row r="221" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A221" s="12" t="s">
         <v>421</v>
       </c>
@@ -20419,7 +20432,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="222" spans="1:27">
+    <row r="222" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A222" s="12" t="s">
         <v>209</v>
       </c>
@@ -20502,7 +20515,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="223" spans="1:27">
+    <row r="223" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A223" s="12" t="s">
         <v>422</v>
       </c>
@@ -20585,7 +20598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="224" spans="1:27">
+    <row r="224" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A224" s="12" t="s">
         <v>423</v>
       </c>
@@ -20668,7 +20681,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="225" spans="1:27">
+    <row r="225" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A225" s="12" t="s">
         <v>425</v>
       </c>
@@ -20751,7 +20764,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="226" spans="1:27">
+    <row r="226" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A226" s="12" t="s">
         <v>426</v>
       </c>
@@ -20834,7 +20847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="227" spans="1:27">
+    <row r="227" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A227" s="12" t="s">
         <v>210</v>
       </c>
@@ -20917,7 +20930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="228" spans="1:27">
+    <row r="228" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A228" s="12" t="s">
         <v>427</v>
       </c>
@@ -21000,7 +21013,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="229" spans="1:27">
+    <row r="229" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A229" s="12" t="s">
         <v>211</v>
       </c>
@@ -21083,7 +21096,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="230" spans="1:27">
+    <row r="230" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A230" s="12" t="s">
         <v>212</v>
       </c>
@@ -21166,7 +21179,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="231" spans="1:27">
+    <row r="231" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A231" s="12" t="s">
         <v>213</v>
       </c>
@@ -21249,7 +21262,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="232" spans="1:27">
+    <row r="232" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A232" s="12" t="s">
         <v>214</v>
       </c>
@@ -21332,7 +21345,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="233" spans="1:27">
+    <row r="233" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A233" s="12" t="s">
         <v>428</v>
       </c>
@@ -21415,7 +21428,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="234" spans="1:27">
+    <row r="234" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A234" s="12" t="s">
         <v>215</v>
       </c>
@@ -21498,7 +21511,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="235" spans="1:27">
+    <row r="235" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A235" s="12" t="s">
         <v>429</v>
       </c>
@@ -21581,7 +21594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="236" spans="1:27">
+    <row r="236" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A236" s="12" t="s">
         <v>216</v>
       </c>
@@ -21664,7 +21677,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="237" spans="1:27">
+    <row r="237" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A237" s="12" t="s">
         <v>217</v>
       </c>
@@ -21747,7 +21760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="238" spans="1:27">
+    <row r="238" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A238" s="12" t="s">
         <v>218</v>
       </c>
@@ -21830,7 +21843,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="239" spans="1:27">
+    <row r="239" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A239" s="12" t="s">
         <v>219</v>
       </c>
@@ -21913,7 +21926,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="240" spans="1:27">
+    <row r="240" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A240" s="12" t="s">
         <v>220</v>
       </c>
@@ -21996,7 +22009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="241" spans="1:27">
+    <row r="241" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A241" s="12" t="s">
         <v>222</v>
       </c>
@@ -22079,7 +22092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="242" spans="1:27">
+    <row r="242" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A242" s="12" t="s">
         <v>223</v>
       </c>
@@ -22162,7 +22175,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="243" spans="1:27">
+    <row r="243" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A243" s="12" t="s">
         <v>224</v>
       </c>
@@ -22245,7 +22258,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="244" spans="1:27">
+    <row r="244" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A244" s="12" t="s">
         <v>430</v>
       </c>
@@ -22328,7 +22341,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="245" spans="1:27">
+    <row r="245" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A245" s="12" t="s">
         <v>431</v>
       </c>
@@ -22411,7 +22424,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="246" spans="1:27">
+    <row r="246" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A246" s="12" t="s">
         <v>225</v>
       </c>
@@ -22494,7 +22507,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="247" spans="1:27">
+    <row r="247" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A247" s="12" t="s">
         <v>226</v>
       </c>
@@ -22577,7 +22590,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="248" spans="1:27">
+    <row r="248" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A248" s="12" t="s">
         <v>227</v>
       </c>
@@ -22660,7 +22673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="249" spans="1:27">
+    <row r="249" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A249" s="12" t="s">
         <v>228</v>
       </c>
@@ -22743,7 +22756,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="250" spans="1:27">
+    <row r="250" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A250" s="12" t="s">
         <v>229</v>
       </c>
@@ -22826,7 +22839,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="251" spans="1:27">
+    <row r="251" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A251" s="12" t="s">
         <v>230</v>
       </c>
@@ -22909,7 +22922,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="252" spans="1:27">
+    <row r="252" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A252" s="12" t="s">
         <v>231</v>
       </c>
@@ -22992,7 +23005,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="253" spans="1:27">
+    <row r="253" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A253" s="12" t="s">
         <v>232</v>
       </c>
@@ -23075,7 +23088,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="254" spans="1:27">
+    <row r="254" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A254" s="12" t="s">
         <v>234</v>
       </c>
@@ -23158,7 +23171,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="255" spans="1:27">
+    <row r="255" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A255" s="12" t="s">
         <v>235</v>
       </c>
@@ -23241,7 +23254,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="256" spans="1:27">
+    <row r="256" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A256" s="12" t="s">
         <v>236</v>
       </c>
@@ -23324,7 +23337,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="257" spans="1:27">
+    <row r="257" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A257" s="12" t="s">
         <v>237</v>
       </c>
@@ -23407,7 +23420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="258" spans="1:27">
+    <row r="258" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A258" s="12" t="s">
         <v>238</v>
       </c>
@@ -23490,7 +23503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="259" spans="1:27" s="3" customFormat="1" ht="50">
+    <row r="259" spans="1:27" s="3" customFormat="1" ht="73.5" x14ac:dyDescent="0.25">
       <c r="A259" s="4" t="s">
         <v>61</v>
       </c>
@@ -23573,7 +23586,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="260" spans="1:27">
+    <row r="260" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A260" s="12" t="s">
         <v>239</v>
       </c>
@@ -23656,7 +23669,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="261" spans="1:27">
+    <row r="261" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A261" s="12" t="s">
         <v>240</v>
       </c>
@@ -23739,7 +23752,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="262" spans="1:27">
+    <row r="262" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A262" s="12" t="s">
         <v>241</v>
       </c>
@@ -23822,7 +23835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="263" spans="1:27">
+    <row r="263" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A263" s="12" t="s">
         <v>242</v>
       </c>
@@ -23905,7 +23918,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="264" spans="1:27">
+    <row r="264" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A264" s="12" t="s">
         <v>243</v>
       </c>
@@ -23988,7 +24001,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="265" spans="1:27">
+    <row r="265" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A265" s="12" t="s">
         <v>244</v>
       </c>
@@ -24071,7 +24084,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="266" spans="1:27">
+    <row r="266" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A266" s="12" t="s">
         <v>245</v>
       </c>
@@ -24154,7 +24167,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="267" spans="1:27">
+    <row r="267" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A267" s="12" t="s">
         <v>246</v>
       </c>
@@ -24237,7 +24250,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="268" spans="1:27">
+    <row r="268" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A268" s="12" t="s">
         <v>247</v>
       </c>
@@ -24320,7 +24333,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="269" spans="1:27">
+    <row r="269" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A269" s="12" t="s">
         <v>248</v>
       </c>
@@ -24403,7 +24416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="270" spans="1:27">
+    <row r="270" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A270" s="12" t="s">
         <v>249</v>
       </c>
@@ -24486,7 +24499,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="271" spans="1:27">
+    <row r="271" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A271" s="12" t="s">
         <v>250</v>
       </c>
@@ -24569,7 +24582,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="272" spans="1:27">
+    <row r="272" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A272" s="12" t="s">
         <v>251</v>
       </c>
@@ -24652,7 +24665,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="273" spans="1:27">
+    <row r="273" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A273" s="12" t="s">
         <v>357</v>
       </c>
@@ -24735,7 +24748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="274" spans="1:27">
+    <row r="274" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A274" s="12" t="s">
         <v>381</v>
       </c>
@@ -24818,7 +24831,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="275" spans="1:27">
+    <row r="275" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A275" s="12" t="s">
         <v>382</v>
       </c>
@@ -24901,7 +24914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="276" spans="1:27">
+    <row r="276" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A276" s="12" t="s">
         <v>383</v>
       </c>
@@ -24984,7 +24997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="277" spans="1:27">
+    <row r="277" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A277" s="12" t="s">
         <v>384</v>
       </c>
@@ -25067,7 +25080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="278" spans="1:27">
+    <row r="278" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A278" s="12" t="s">
         <v>97</v>
       </c>
@@ -25150,7 +25163,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="279" spans="1:27">
+    <row r="279" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A279" s="12" t="s">
         <v>106</v>
       </c>
@@ -25233,7 +25246,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="280" spans="1:27">
+    <row r="280" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A280" s="12" t="s">
         <v>112</v>
       </c>
@@ -25316,7 +25329,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="281" spans="1:27">
+    <row r="281" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A281" s="12" t="s">
         <v>117</v>
       </c>
@@ -25399,7 +25412,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="282" spans="1:27">
+    <row r="282" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A282" s="12" t="s">
         <v>125</v>
       </c>
@@ -25482,7 +25495,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="283" spans="1:27">
+    <row r="283" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A283" s="12" t="s">
         <v>132</v>
       </c>
@@ -25565,7 +25578,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="284" spans="1:27">
+    <row r="284" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A284" s="12" t="s">
         <v>165</v>
       </c>
@@ -25648,7 +25661,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="285" spans="1:27">
+    <row r="285" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A285" s="12" t="s">
         <v>185</v>
       </c>
@@ -25731,7 +25744,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="286" spans="1:27">
+    <row r="286" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A286" s="12" t="s">
         <v>186</v>
       </c>
@@ -25814,7 +25827,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="287" spans="1:27">
+    <row r="287" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A287" s="12" t="s">
         <v>62</v>
       </c>
@@ -25897,7 +25910,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="288" spans="1:27">
+    <row r="288" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A288" s="12" t="s">
         <v>63</v>
       </c>
@@ -25980,7 +25993,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="289" spans="1:27">
+    <row r="289" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A289" s="12" t="s">
         <v>187</v>
       </c>
@@ -26063,7 +26076,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="290" spans="1:27">
+    <row r="290" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A290" s="12" t="s">
         <v>64</v>
       </c>
@@ -26146,7 +26159,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="291" spans="1:27">
+    <row r="291" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A291" s="12" t="s">
         <v>65</v>
       </c>
@@ -26229,7 +26242,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="292" spans="1:27">
+    <row r="292" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A292" s="12" t="s">
         <v>188</v>
       </c>
@@ -26312,7 +26325,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="293" spans="1:27">
+    <row r="293" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A293" s="12" t="s">
         <v>189</v>
       </c>
@@ -26395,7 +26408,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="294" spans="1:27">
+    <row r="294" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A294" s="12" t="s">
         <v>190</v>
       </c>
@@ -26478,7 +26491,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="295" spans="1:27">
+    <row r="295" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A295" s="12" t="s">
         <v>193</v>
       </c>
@@ -26561,7 +26574,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="296" spans="1:27">
+    <row r="296" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A296" s="12" t="s">
         <v>184</v>
       </c>
@@ -26644,7 +26657,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="297" spans="1:27">
+    <row r="297" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A297" s="12" t="s">
         <v>195</v>
       </c>
@@ -26727,7 +26740,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="298" spans="1:27">
+    <row r="298" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A298" s="12" t="s">
         <v>68</v>
       </c>
@@ -26810,7 +26823,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="299" spans="1:27">
+    <row r="299" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A299" s="12" t="s">
         <v>69</v>
       </c>
@@ -26893,7 +26906,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="300" spans="1:27">
+    <row r="300" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A300" s="12" t="s">
         <v>70</v>
       </c>
@@ -26976,7 +26989,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="301" spans="1:27">
+    <row r="301" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A301" s="12" t="s">
         <v>71</v>
       </c>
@@ -27059,7 +27072,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="302" spans="1:27" s="3" customFormat="1" ht="50">
+    <row r="302" spans="1:27" s="3" customFormat="1" ht="73.5" x14ac:dyDescent="0.25">
       <c r="A302" s="4" t="s">
         <v>61</v>
       </c>
@@ -27142,7 +27155,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="303" spans="1:27">
+    <row r="303" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A303" s="12" t="s">
         <v>196</v>
       </c>
@@ -27225,7 +27238,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="304" spans="1:27">
+    <row r="304" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A304" s="12" t="s">
         <v>72</v>
       </c>
@@ -27308,7 +27321,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="305" spans="1:27">
+    <row r="305" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A305" s="12" t="s">
         <v>197</v>
       </c>
@@ -27391,7 +27404,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="306" spans="1:27">
+    <row r="306" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A306" s="12" t="s">
         <v>73</v>
       </c>
@@ -27474,7 +27487,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="307" spans="1:27">
+    <row r="307" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A307" s="12" t="s">
         <v>74</v>
       </c>
@@ -27557,7 +27570,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="308" spans="1:27">
+    <row r="308" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A308" s="12" t="s">
         <v>76</v>
       </c>
@@ -27640,7 +27653,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="309" spans="1:27">
+    <row r="309" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A309" s="12" t="s">
         <v>77</v>
       </c>
@@ -27723,7 +27736,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="310" spans="1:27">
+    <row r="310" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A310" s="12" t="s">
         <v>79</v>
       </c>
@@ -27806,7 +27819,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="311" spans="1:27">
+    <row r="311" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A311" s="12" t="s">
         <v>80</v>
       </c>
@@ -27889,7 +27902,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="312" spans="1:27">
+    <row r="312" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A312" s="12" t="s">
         <v>81</v>
       </c>
@@ -27972,7 +27985,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="313" spans="1:27">
+    <row r="313" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A313" s="12" t="s">
         <v>82</v>
       </c>
@@ -28055,7 +28068,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="314" spans="1:27">
+    <row r="314" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A314" s="12" t="s">
         <v>199</v>
       </c>
@@ -28138,7 +28151,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="315" spans="1:27">
+    <row r="315" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A315" s="12" t="s">
         <v>83</v>
       </c>
@@ -28221,7 +28234,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="316" spans="1:27">
+    <row r="316" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A316" s="12" t="s">
         <v>84</v>
       </c>
@@ -28304,7 +28317,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="317" spans="1:27">
+    <row r="317" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A317" s="12" t="s">
         <v>85</v>
       </c>
@@ -28387,7 +28400,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="318" spans="1:27">
+    <row r="318" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A318" s="12" t="s">
         <v>86</v>
       </c>
@@ -28470,7 +28483,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="319" spans="1:27">
+    <row r="319" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A319" s="12" t="s">
         <v>87</v>
       </c>
@@ -28553,7 +28566,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="320" spans="1:27">
+    <row r="320" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A320" s="12" t="s">
         <v>202</v>
       </c>
@@ -28636,7 +28649,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="321" spans="1:27">
+    <row r="321" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A321" s="12" t="s">
         <v>313</v>
       </c>
@@ -28719,7 +28732,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="322" spans="1:27">
+    <row r="322" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A322" s="12" t="s">
         <v>349</v>
       </c>
@@ -28802,7 +28815,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="323" spans="1:27">
+    <row r="323" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A323" s="12" t="s">
         <v>314</v>
       </c>
@@ -28885,7 +28898,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="324" spans="1:27">
+    <row r="324" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A324" s="12" t="s">
         <v>315</v>
       </c>
@@ -28968,7 +28981,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="325" spans="1:27">
+    <row r="325" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A325" s="12" t="s">
         <v>316</v>
       </c>
@@ -29051,7 +29064,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="326" spans="1:27">
+    <row r="326" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A326" s="12" t="s">
         <v>317</v>
       </c>
@@ -29134,7 +29147,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="327" spans="1:27">
+    <row r="327" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A327" s="12" t="s">
         <v>318</v>
       </c>
@@ -29217,7 +29230,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="328" spans="1:27">
+    <row r="328" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A328" s="12" t="s">
         <v>319</v>
       </c>
@@ -29300,7 +29313,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="329" spans="1:27">
+    <row r="329" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A329" s="12" t="s">
         <v>320</v>
       </c>
@@ -29383,7 +29396,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="330" spans="1:27">
+    <row r="330" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A330" s="12" t="s">
         <v>321</v>
       </c>
@@ -29466,7 +29479,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="331" spans="1:27">
+    <row r="331" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A331" s="12" t="s">
         <v>322</v>
       </c>
@@ -29549,7 +29562,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="332" spans="1:27">
+    <row r="332" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A332" s="12" t="s">
         <v>323</v>
       </c>
@@ -29632,7 +29645,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="333" spans="1:27">
+    <row r="333" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A333" s="12" t="s">
         <v>324</v>
       </c>
@@ -29715,7 +29728,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="334" spans="1:27">
+    <row r="334" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A334" s="12" t="s">
         <v>325</v>
       </c>
@@ -29798,7 +29811,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="335" spans="1:27">
+    <row r="335" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A335" s="12" t="s">
         <v>326</v>
       </c>
@@ -29881,7 +29894,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="336" spans="1:27">
+    <row r="336" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A336" s="12" t="s">
         <v>327</v>
       </c>
@@ -29964,7 +29977,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="337" spans="1:27">
+    <row r="337" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A337" s="12" t="s">
         <v>330</v>
       </c>
@@ -30047,7 +30060,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="338" spans="1:27">
+    <row r="338" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A338" s="12" t="s">
         <v>333</v>
       </c>
@@ -30130,7 +30143,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="339" spans="1:27">
+    <row r="339" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A339" s="12" t="s">
         <v>336</v>
       </c>
@@ -30213,7 +30226,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="340" spans="1:27">
+    <row r="340" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A340" s="12" t="s">
         <v>280</v>
       </c>
@@ -30296,7 +30309,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="341" spans="1:27">
+    <row r="341" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A341" s="12" t="s">
         <v>281</v>
       </c>
@@ -30379,7 +30392,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="342" spans="1:27">
+    <row r="342" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A342" s="12" t="s">
         <v>282</v>
       </c>
@@ -30462,7 +30475,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="343" spans="1:27">
+    <row r="343" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A343" s="12" t="s">
         <v>286</v>
       </c>
@@ -30545,7 +30558,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="344" spans="1:27">
+    <row r="344" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A344" s="12" t="s">
         <v>287</v>
       </c>
@@ -30628,7 +30641,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="345" spans="1:27" s="3" customFormat="1" ht="50">
+    <row r="345" spans="1:27" s="3" customFormat="1" ht="73.5" x14ac:dyDescent="0.25">
       <c r="A345" s="4" t="s">
         <v>61</v>
       </c>
@@ -30711,7 +30724,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="346" spans="1:27">
+    <row r="346" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A346" s="12" t="s">
         <v>295</v>
       </c>
@@ -30794,628 +30807,628 @@
         <v>406</v>
       </c>
     </row>
-    <row r="347" spans="1:27">
+    <row r="347" spans="1:27" x14ac:dyDescent="0.25">
       <c r="X347" s="2"/>
     </row>
-    <row r="348" spans="1:27">
+    <row r="348" spans="1:27" x14ac:dyDescent="0.25">
       <c r="X348" s="2"/>
     </row>
-    <row r="349" spans="1:27">
+    <row r="349" spans="1:27" x14ac:dyDescent="0.25">
       <c r="X349" s="2"/>
     </row>
-    <row r="350" spans="1:27">
+    <row r="350" spans="1:27" x14ac:dyDescent="0.25">
       <c r="X350" s="2"/>
     </row>
-    <row r="351" spans="1:27">
+    <row r="351" spans="1:27" x14ac:dyDescent="0.25">
       <c r="X351" s="2"/>
     </row>
-    <row r="352" spans="1:27">
+    <row r="352" spans="1:27" x14ac:dyDescent="0.25">
       <c r="X352" s="2"/>
     </row>
-    <row r="353" spans="24:24">
+    <row r="353" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X353" s="2"/>
     </row>
-    <row r="354" spans="24:24">
+    <row r="354" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X354" s="2"/>
     </row>
-    <row r="355" spans="24:24">
+    <row r="355" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X355" s="2"/>
     </row>
-    <row r="356" spans="24:24">
+    <row r="356" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X356" s="2"/>
     </row>
-    <row r="357" spans="24:24">
+    <row r="357" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X357" s="2"/>
     </row>
-    <row r="358" spans="24:24">
+    <row r="358" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X358" s="2"/>
     </row>
-    <row r="359" spans="24:24">
+    <row r="359" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X359" s="2"/>
     </row>
-    <row r="360" spans="24:24">
+    <row r="360" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X360" s="2"/>
     </row>
-    <row r="361" spans="24:24">
+    <row r="361" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X361" s="2"/>
     </row>
-    <row r="362" spans="24:24">
+    <row r="362" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X362" s="2"/>
     </row>
-    <row r="363" spans="24:24">
+    <row r="363" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X363" s="2"/>
     </row>
-    <row r="364" spans="24:24">
+    <row r="364" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X364" s="2"/>
     </row>
-    <row r="365" spans="24:24">
+    <row r="365" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X365" s="2"/>
     </row>
-    <row r="366" spans="24:24">
+    <row r="366" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X366" s="2"/>
     </row>
-    <row r="367" spans="24:24">
+    <row r="367" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X367" s="2"/>
     </row>
-    <row r="368" spans="24:24">
+    <row r="368" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X368" s="2"/>
     </row>
-    <row r="369" spans="24:24">
+    <row r="369" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X369" s="2"/>
     </row>
-    <row r="370" spans="24:24">
+    <row r="370" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X370" s="2"/>
     </row>
-    <row r="371" spans="24:24">
+    <row r="371" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X371" s="2"/>
     </row>
-    <row r="372" spans="24:24">
+    <row r="372" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X372" s="2"/>
     </row>
-    <row r="373" spans="24:24">
+    <row r="373" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X373" s="2"/>
     </row>
-    <row r="374" spans="24:24">
+    <row r="374" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X374" s="2"/>
     </row>
-    <row r="375" spans="24:24">
+    <row r="375" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X375" s="2"/>
     </row>
-    <row r="376" spans="24:24">
+    <row r="376" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X376" s="2"/>
     </row>
-    <row r="377" spans="24:24">
+    <row r="377" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X377" s="2"/>
     </row>
-    <row r="378" spans="24:24">
+    <row r="378" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X378" s="2"/>
     </row>
-    <row r="379" spans="24:24">
+    <row r="379" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X379" s="2"/>
     </row>
-    <row r="380" spans="24:24">
+    <row r="380" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X380" s="2"/>
     </row>
-    <row r="381" spans="24:24">
+    <row r="381" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X381" s="2"/>
     </row>
-    <row r="382" spans="24:24">
+    <row r="382" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X382" s="2"/>
     </row>
-    <row r="383" spans="24:24">
+    <row r="383" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X383" s="2"/>
     </row>
-    <row r="384" spans="24:24">
+    <row r="384" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X384" s="2"/>
     </row>
-    <row r="385" spans="24:24">
+    <row r="385" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X385" s="2"/>
     </row>
-    <row r="386" spans="24:24">
+    <row r="386" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X386" s="2"/>
     </row>
-    <row r="387" spans="24:24">
+    <row r="387" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X387" s="2"/>
     </row>
-    <row r="388" spans="24:24">
+    <row r="388" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X388" s="2"/>
     </row>
-    <row r="389" spans="24:24">
+    <row r="389" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X389" s="2"/>
     </row>
-    <row r="390" spans="24:24">
+    <row r="390" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X390" s="2"/>
     </row>
-    <row r="391" spans="24:24">
+    <row r="391" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X391" s="2"/>
     </row>
-    <row r="392" spans="24:24">
+    <row r="392" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X392" s="2"/>
     </row>
-    <row r="393" spans="24:24">
+    <row r="393" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X393" s="2"/>
     </row>
-    <row r="394" spans="24:24">
+    <row r="394" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X394" s="2"/>
     </row>
-    <row r="395" spans="24:24">
+    <row r="395" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X395" s="2"/>
     </row>
-    <row r="396" spans="24:24">
+    <row r="396" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X396" s="2"/>
     </row>
-    <row r="397" spans="24:24">
+    <row r="397" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X397" s="2"/>
     </row>
-    <row r="398" spans="24:24">
+    <row r="398" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X398" s="2"/>
     </row>
-    <row r="399" spans="24:24">
+    <row r="399" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X399" s="2"/>
     </row>
-    <row r="400" spans="24:24">
+    <row r="400" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X400" s="2"/>
     </row>
-    <row r="401" spans="24:24">
+    <row r="401" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X401" s="2"/>
     </row>
-    <row r="402" spans="24:24">
+    <row r="402" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X402" s="2"/>
     </row>
-    <row r="403" spans="24:24">
+    <row r="403" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X403" s="2"/>
     </row>
-    <row r="404" spans="24:24">
+    <row r="404" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X404" s="2"/>
     </row>
-    <row r="405" spans="24:24">
+    <row r="405" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X405" s="2"/>
     </row>
-    <row r="406" spans="24:24">
+    <row r="406" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X406" s="2"/>
     </row>
-    <row r="407" spans="24:24">
+    <row r="407" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X407" s="2"/>
     </row>
-    <row r="408" spans="24:24">
+    <row r="408" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X408" s="2"/>
     </row>
-    <row r="409" spans="24:24">
+    <row r="409" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X409" s="2"/>
     </row>
-    <row r="410" spans="24:24">
+    <row r="410" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X410" s="2"/>
     </row>
-    <row r="411" spans="24:24">
+    <row r="411" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X411" s="2"/>
     </row>
-    <row r="412" spans="24:24">
+    <row r="412" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X412" s="2"/>
     </row>
-    <row r="413" spans="24:24">
+    <row r="413" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X413" s="2"/>
     </row>
-    <row r="414" spans="24:24">
+    <row r="414" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X414" s="2"/>
     </row>
-    <row r="415" spans="24:24">
+    <row r="415" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X415" s="2"/>
     </row>
-    <row r="416" spans="24:24">
+    <row r="416" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X416" s="2"/>
     </row>
-    <row r="417" spans="24:24">
+    <row r="417" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X417" s="2"/>
     </row>
-    <row r="418" spans="24:24">
+    <row r="418" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X418" s="2"/>
     </row>
-    <row r="419" spans="24:24">
+    <row r="419" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X419" s="2"/>
     </row>
-    <row r="420" spans="24:24">
+    <row r="420" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X420" s="2"/>
     </row>
-    <row r="421" spans="24:24">
+    <row r="421" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X421" s="2"/>
     </row>
-    <row r="422" spans="24:24">
+    <row r="422" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X422" s="2"/>
     </row>
-    <row r="423" spans="24:24">
+    <row r="423" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X423" s="2"/>
     </row>
-    <row r="424" spans="24:24">
+    <row r="424" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X424" s="2"/>
     </row>
-    <row r="425" spans="24:24">
+    <row r="425" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X425" s="2"/>
     </row>
-    <row r="426" spans="24:24">
+    <row r="426" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X426" s="2"/>
     </row>
-    <row r="427" spans="24:24">
+    <row r="427" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X427" s="2"/>
     </row>
-    <row r="428" spans="24:24">
+    <row r="428" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X428" s="2"/>
     </row>
-    <row r="429" spans="24:24">
+    <row r="429" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X429" s="2"/>
     </row>
-    <row r="430" spans="24:24">
+    <row r="430" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X430" s="2"/>
     </row>
-    <row r="431" spans="24:24">
+    <row r="431" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X431" s="2"/>
     </row>
-    <row r="432" spans="24:24">
+    <row r="432" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X432" s="2"/>
     </row>
-    <row r="433" spans="24:24">
+    <row r="433" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X433" s="2"/>
     </row>
-    <row r="434" spans="24:24">
+    <row r="434" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X434" s="2"/>
     </row>
-    <row r="435" spans="24:24">
+    <row r="435" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X435" s="2"/>
     </row>
-    <row r="436" spans="24:24">
+    <row r="436" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X436" s="2"/>
     </row>
-    <row r="437" spans="24:24">
+    <row r="437" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X437" s="2"/>
     </row>
-    <row r="438" spans="24:24">
+    <row r="438" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X438" s="2"/>
     </row>
-    <row r="439" spans="24:24">
+    <row r="439" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X439" s="2"/>
     </row>
-    <row r="440" spans="24:24">
+    <row r="440" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X440" s="2"/>
     </row>
-    <row r="441" spans="24:24">
+    <row r="441" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X441" s="2"/>
     </row>
-    <row r="442" spans="24:24">
+    <row r="442" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X442" s="2"/>
     </row>
-    <row r="443" spans="24:24">
+    <row r="443" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X443" s="2"/>
     </row>
-    <row r="444" spans="24:24">
+    <row r="444" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X444" s="2"/>
     </row>
-    <row r="445" spans="24:24">
+    <row r="445" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X445" s="2"/>
     </row>
-    <row r="446" spans="24:24">
+    <row r="446" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X446" s="2"/>
     </row>
-    <row r="447" spans="24:24">
+    <row r="447" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X447" s="2"/>
     </row>
-    <row r="448" spans="24:24">
+    <row r="448" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X448" s="2"/>
     </row>
-    <row r="449" spans="24:24">
+    <row r="449" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X449" s="2"/>
     </row>
-    <row r="450" spans="24:24">
+    <row r="450" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X450" s="2"/>
     </row>
-    <row r="451" spans="24:24">
+    <row r="451" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X451" s="2"/>
     </row>
-    <row r="452" spans="24:24">
+    <row r="452" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X452" s="2"/>
     </row>
-    <row r="453" spans="24:24">
+    <row r="453" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X453" s="2"/>
     </row>
-    <row r="454" spans="24:24">
+    <row r="454" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X454" s="2"/>
     </row>
-    <row r="455" spans="24:24">
+    <row r="455" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X455" s="2"/>
     </row>
-    <row r="456" spans="24:24">
+    <row r="456" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X456" s="2"/>
     </row>
-    <row r="457" spans="24:24">
+    <row r="457" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X457" s="2"/>
     </row>
-    <row r="458" spans="24:24">
+    <row r="458" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X458" s="2"/>
     </row>
-    <row r="459" spans="24:24">
+    <row r="459" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X459" s="2"/>
     </row>
-    <row r="460" spans="24:24">
+    <row r="460" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X460" s="2"/>
     </row>
-    <row r="461" spans="24:24">
+    <row r="461" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X461" s="2"/>
     </row>
-    <row r="462" spans="24:24">
+    <row r="462" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X462" s="2"/>
     </row>
-    <row r="463" spans="24:24">
+    <row r="463" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X463" s="2"/>
     </row>
-    <row r="464" spans="24:24">
+    <row r="464" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X464" s="2"/>
     </row>
-    <row r="465" spans="24:24">
+    <row r="465" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X465" s="2"/>
     </row>
-    <row r="466" spans="24:24">
+    <row r="466" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X466" s="2"/>
     </row>
-    <row r="467" spans="24:24">
+    <row r="467" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X467" s="2"/>
     </row>
-    <row r="468" spans="24:24">
+    <row r="468" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X468" s="2"/>
     </row>
-    <row r="469" spans="24:24">
+    <row r="469" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X469" s="2"/>
     </row>
-    <row r="470" spans="24:24">
+    <row r="470" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X470" s="2"/>
     </row>
-    <row r="471" spans="24:24">
+    <row r="471" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X471" s="2"/>
     </row>
-    <row r="472" spans="24:24">
+    <row r="472" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X472" s="2"/>
     </row>
-    <row r="473" spans="24:24">
+    <row r="473" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X473" s="2"/>
     </row>
-    <row r="474" spans="24:24">
+    <row r="474" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X474" s="2"/>
     </row>
-    <row r="475" spans="24:24">
+    <row r="475" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X475" s="2"/>
     </row>
-    <row r="476" spans="24:24">
+    <row r="476" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X476" s="2"/>
     </row>
-    <row r="477" spans="24:24">
+    <row r="477" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X477" s="2"/>
     </row>
-    <row r="478" spans="24:24">
+    <row r="478" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X478" s="2"/>
     </row>
-    <row r="479" spans="24:24">
+    <row r="479" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X479" s="2"/>
     </row>
-    <row r="480" spans="24:24">
+    <row r="480" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X480" s="2"/>
     </row>
-    <row r="481" spans="24:24">
+    <row r="481" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X481" s="2"/>
     </row>
-    <row r="482" spans="24:24">
+    <row r="482" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X482" s="2"/>
     </row>
-    <row r="483" spans="24:24">
+    <row r="483" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X483" s="2"/>
     </row>
-    <row r="484" spans="24:24">
+    <row r="484" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X484" s="2"/>
     </row>
-    <row r="485" spans="24:24">
+    <row r="485" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X485" s="2"/>
     </row>
-    <row r="486" spans="24:24">
+    <row r="486" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X486" s="2"/>
     </row>
-    <row r="487" spans="24:24">
+    <row r="487" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X487" s="2"/>
     </row>
-    <row r="488" spans="24:24">
+    <row r="488" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X488" s="2"/>
     </row>
-    <row r="489" spans="24:24">
+    <row r="489" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X489" s="2"/>
     </row>
-    <row r="490" spans="24:24">
+    <row r="490" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X490" s="2"/>
     </row>
-    <row r="491" spans="24:24">
+    <row r="491" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X491" s="2"/>
     </row>
-    <row r="492" spans="24:24">
+    <row r="492" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X492" s="2"/>
     </row>
-    <row r="493" spans="24:24">
+    <row r="493" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X493" s="2"/>
     </row>
-    <row r="494" spans="24:24">
+    <row r="494" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X494" s="2"/>
     </row>
-    <row r="495" spans="24:24">
+    <row r="495" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X495" s="2"/>
     </row>
-    <row r="496" spans="24:24">
+    <row r="496" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X496" s="2"/>
     </row>
-    <row r="497" spans="24:24">
+    <row r="497" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X497" s="2"/>
     </row>
-    <row r="498" spans="24:24">
+    <row r="498" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X498" s="2"/>
     </row>
-    <row r="499" spans="24:24">
+    <row r="499" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X499" s="2"/>
     </row>
-    <row r="500" spans="24:24">
+    <row r="500" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X500" s="2"/>
     </row>
-    <row r="501" spans="24:24">
+    <row r="501" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X501" s="2"/>
     </row>
-    <row r="502" spans="24:24">
+    <row r="502" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X502" s="2"/>
     </row>
-    <row r="503" spans="24:24">
+    <row r="503" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X503" s="2"/>
     </row>
-    <row r="504" spans="24:24">
+    <row r="504" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X504" s="2"/>
     </row>
-    <row r="505" spans="24:24">
+    <row r="505" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X505" s="2"/>
     </row>
-    <row r="506" spans="24:24">
+    <row r="506" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X506" s="2"/>
     </row>
-    <row r="507" spans="24:24">
+    <row r="507" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X507" s="2"/>
     </row>
-    <row r="508" spans="24:24">
+    <row r="508" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X508" s="2"/>
     </row>
-    <row r="509" spans="24:24">
+    <row r="509" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X509" s="2"/>
     </row>
-    <row r="510" spans="24:24">
+    <row r="510" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X510" s="2"/>
     </row>
-    <row r="511" spans="24:24">
+    <row r="511" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X511" s="2"/>
     </row>
-    <row r="512" spans="24:24">
+    <row r="512" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X512" s="2"/>
     </row>
-    <row r="513" spans="24:24">
+    <row r="513" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X513" s="2"/>
     </row>
-    <row r="514" spans="24:24">
+    <row r="514" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X514" s="2"/>
     </row>
-    <row r="515" spans="24:24">
+    <row r="515" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X515" s="2"/>
     </row>
-    <row r="516" spans="24:24">
+    <row r="516" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X516" s="2"/>
     </row>
-    <row r="517" spans="24:24">
+    <row r="517" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X517" s="2"/>
     </row>
-    <row r="518" spans="24:24">
+    <row r="518" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X518" s="2"/>
     </row>
-    <row r="519" spans="24:24">
+    <row r="519" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X519" s="2"/>
     </row>
-    <row r="520" spans="24:24">
+    <row r="520" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X520" s="2"/>
     </row>
-    <row r="521" spans="24:24">
+    <row r="521" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X521" s="2"/>
     </row>
-    <row r="522" spans="24:24">
+    <row r="522" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X522" s="2"/>
     </row>
-    <row r="523" spans="24:24">
+    <row r="523" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X523" s="2"/>
     </row>
-    <row r="524" spans="24:24">
+    <row r="524" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X524" s="2"/>
     </row>
-    <row r="525" spans="24:24">
+    <row r="525" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X525" s="2"/>
     </row>
-    <row r="526" spans="24:24">
+    <row r="526" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X526" s="2"/>
     </row>
-    <row r="527" spans="24:24">
+    <row r="527" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X527" s="2"/>
     </row>
-    <row r="528" spans="24:24">
+    <row r="528" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X528" s="2"/>
     </row>
-    <row r="529" spans="24:24">
+    <row r="529" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X529" s="2"/>
     </row>
-    <row r="530" spans="24:24">
+    <row r="530" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X530" s="2"/>
     </row>
-    <row r="531" spans="24:24">
+    <row r="531" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X531" s="2"/>
     </row>
-    <row r="532" spans="24:24">
+    <row r="532" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X532" s="2"/>
     </row>
-    <row r="533" spans="24:24">
+    <row r="533" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X533" s="2"/>
     </row>
-    <row r="534" spans="24:24">
+    <row r="534" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X534" s="2"/>
     </row>
-    <row r="535" spans="24:24">
+    <row r="535" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X535" s="2"/>
     </row>
-    <row r="536" spans="24:24">
+    <row r="536" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X536" s="2"/>
     </row>
-    <row r="537" spans="24:24">
+    <row r="537" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X537" s="2"/>
     </row>
-    <row r="538" spans="24:24">
+    <row r="538" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X538" s="2"/>
     </row>
-    <row r="539" spans="24:24">
+    <row r="539" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X539" s="2"/>
     </row>
-    <row r="540" spans="24:24">
+    <row r="540" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X540" s="2"/>
     </row>
-    <row r="541" spans="24:24">
+    <row r="541" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X541" s="2"/>
     </row>
-    <row r="542" spans="24:24">
+    <row r="542" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X542" s="2"/>
     </row>
-    <row r="543" spans="24:24">
+    <row r="543" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X543" s="2"/>
     </row>
-    <row r="544" spans="24:24">
+    <row r="544" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X544" s="2"/>
     </row>
-    <row r="545" spans="24:24">
+    <row r="545" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X545" s="2"/>
     </row>
-    <row r="546" spans="24:24">
+    <row r="546" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X546" s="2"/>
     </row>
-    <row r="547" spans="24:24">
+    <row r="547" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X547" s="2"/>
     </row>
-    <row r="548" spans="24:24">
+    <row r="548" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X548" s="2"/>
     </row>
-    <row r="549" spans="24:24">
+    <row r="549" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X549" s="2"/>
     </row>
-    <row r="550" spans="24:24">
+    <row r="550" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X550" s="2"/>
     </row>
-    <row r="551" spans="24:24">
+    <row r="551" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X551" s="2"/>
     </row>
-    <row r="552" spans="24:24">
+    <row r="552" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X552" s="2"/>
     </row>
-    <row r="553" spans="24:24">
+    <row r="553" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X553" s="2"/>
     </row>
-    <row r="554" spans="24:24">
+    <row r="554" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X554" s="2"/>
     </row>
   </sheetData>

</xml_diff>